<commit_message>
US 2025 FIRST UPDATE
</commit_message>
<xml_diff>
--- a/public/assets/file/format_anggota_kelompok_last.xlsx
+++ b/public/assets/file/format_anggota_kelompok_last.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>username</t>
   </si>
@@ -191,6 +191,9 @@
     <t>R. 48</t>
   </si>
   <si>
+    <t>R.COBA</t>
+  </si>
+  <si>
     <t>X AKL 1</t>
   </si>
   <si>
@@ -333,6 +336,9 @@
   </si>
   <si>
     <t>XI MPL 3</t>
+  </si>
+  <si>
+    <t>coba</t>
   </si>
 </sst>
 </file>
@@ -758,7 +764,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C6" sqref="C6"/>
@@ -824,7 +830,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -838,7 +844,7 @@
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -852,7 +858,7 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -860,7 +866,7 @@
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -868,7 +874,7 @@
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -876,7 +882,7 @@
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -884,7 +890,7 @@
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -892,7 +898,7 @@
         <v>17</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -900,7 +906,7 @@
         <v>18</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -908,7 +914,7 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -916,7 +922,7 @@
         <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -924,7 +930,7 @@
         <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -932,7 +938,7 @@
         <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -940,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -948,7 +954,7 @@
         <v>24</v>
       </c>
       <c r="J17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -956,7 +962,7 @@
         <v>25</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -964,7 +970,7 @@
         <v>26</v>
       </c>
       <c r="J19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -972,7 +978,7 @@
         <v>27</v>
       </c>
       <c r="J20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -980,7 +986,7 @@
         <v>28</v>
       </c>
       <c r="J21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -988,7 +994,7 @@
         <v>29</v>
       </c>
       <c r="J22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -996,7 +1002,7 @@
         <v>30</v>
       </c>
       <c r="J23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1004,7 +1010,7 @@
         <v>31</v>
       </c>
       <c r="J24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1012,7 +1018,7 @@
         <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1020,7 +1026,7 @@
         <v>33</v>
       </c>
       <c r="J26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1028,7 +1034,7 @@
         <v>34</v>
       </c>
       <c r="J27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1036,7 +1042,7 @@
         <v>35</v>
       </c>
       <c r="J28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1044,7 +1050,7 @@
         <v>36</v>
       </c>
       <c r="J29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1052,7 +1058,7 @@
         <v>37</v>
       </c>
       <c r="J30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1060,7 +1066,7 @@
         <v>38</v>
       </c>
       <c r="J31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1068,7 +1074,7 @@
         <v>39</v>
       </c>
       <c r="J32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1076,7 +1082,7 @@
         <v>40</v>
       </c>
       <c r="J33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1084,7 +1090,7 @@
         <v>41</v>
       </c>
       <c r="J34" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1092,7 +1098,7 @@
         <v>42</v>
       </c>
       <c r="J35" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1100,7 +1106,7 @@
         <v>43</v>
       </c>
       <c r="J36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1108,7 +1114,7 @@
         <v>44</v>
       </c>
       <c r="J37" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1116,7 +1122,7 @@
         <v>45</v>
       </c>
       <c r="J38" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1124,7 +1130,7 @@
         <v>46</v>
       </c>
       <c r="J39" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1132,7 +1138,7 @@
         <v>47</v>
       </c>
       <c r="J40" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1140,7 +1146,7 @@
         <v>48</v>
       </c>
       <c r="J41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1148,7 +1154,7 @@
         <v>49</v>
       </c>
       <c r="J42" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1156,7 +1162,7 @@
         <v>50</v>
       </c>
       <c r="J43" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1164,7 +1170,7 @@
         <v>51</v>
       </c>
       <c r="J44" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1172,7 +1178,7 @@
         <v>52</v>
       </c>
       <c r="J45" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1180,7 +1186,7 @@
         <v>53</v>
       </c>
       <c r="J46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -1188,7 +1194,7 @@
         <v>54</v>
       </c>
       <c r="J47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1196,7 +1202,7 @@
         <v>55</v>
       </c>
       <c r="J48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -1204,7 +1210,7 @@
         <v>56</v>
       </c>
       <c r="J49" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -1212,7 +1218,15 @@
         <v>57</v>
       </c>
       <c r="J50" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="I51" t="s">
+        <v>58</v>
+      </c>
+      <c r="J51" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>